<commit_message>
add yfinance and add to dataset
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28428B91-D138-437A-A99E-6BD7741C9EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B714867-65A5-4A1D-8DCF-27E64A476D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="1545" windowWidth="21120" windowHeight="13140" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>File/Line</t>
   </si>
@@ -81,18 +81,12 @@
     <t xml:space="preserve">utilize Heroku </t>
   </si>
   <si>
-    <t>/ SQL postgres to store</t>
-  </si>
-  <si>
     <t>run on portfolio</t>
   </si>
   <si>
     <t>Analysis release</t>
   </si>
   <si>
-    <t>Digital Ocean</t>
-  </si>
-  <si>
     <t>Task/M</t>
   </si>
   <si>
@@ -100,13 +94,43 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>https://stackabuse.com/adding-a-postgresql-database-to-a-node-js-app-on-heroku/</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/airflow-how-to-refresh-stocks-data-while-you-sleep-part-1-a464514e45b7</t>
+  </si>
+  <si>
+    <t>Comment2</t>
+  </si>
+  <si>
+    <t>/ SQL postgres w JSON to store</t>
+  </si>
+  <si>
+    <t>https://github.com/lsclovecode/Real-Time-Stock-Streaming-Pipeline</t>
+  </si>
+  <si>
+    <t>Comment3</t>
+  </si>
+  <si>
+    <t>Digital Ocean / Google Cloud Kubernetes</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/sql</t>
+  </si>
+  <si>
+    <t>https://dev.to/kenessajr/deploy-a-react-app-to-digitalocean-using-github-actions-and-docker-4pln</t>
+  </si>
+  <si>
+    <t>https://github.com/romanorac/pandas-analytics-server</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +142,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,10 +178,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -172,8 +205,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -486,13 +523,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E7739-8A07-4817-ADF7-CBF975C125FD}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -506,16 +543,18 @@
     <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="31.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
@@ -541,8 +580,14 @@
       <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.1</v>
       </c>
@@ -554,7 +599,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="F2" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E2)),"Closed",IF(NOT(ISBLANK(D2)),"In Progress",""))</f>
+        <f t="shared" ref="F2:F25" si="0">IF(NOT(ISBLANK(E2)),"Closed",IF(NOT(ISBLANK(D2)),"In Progress",""))</f>
         <v/>
       </c>
       <c r="H2" s="1" t="s">
@@ -564,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -574,10 +619,12 @@
       <c r="C3" s="4">
         <v>44162</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>44180</v>
+      </c>
       <c r="F3" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E3)),"Closed",IF(NOT(ISBLANK(D3)),"In Progress",""))</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>In Progress</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
@@ -586,7 +633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.1</v>
       </c>
@@ -598,36 +645,36 @@
       </c>
       <c r="D4" s="4"/>
       <c r="F4" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E4)),"Closed",IF(NOT(ISBLANK(D4)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6">
         <v>44136</v>
       </c>
       <c r="F5" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E5)),"Closed",IF(NOT(ISBLANK(D5)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v>In Progress</v>
       </c>
       <c r="G5" s="6">
         <v>44196</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.2</v>
       </c>
@@ -639,7 +686,7 @@
       </c>
       <c r="D6" s="4"/>
       <c r="F6" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E6)),"Closed",IF(NOT(ISBLANK(D6)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H6" s="1" t="s">
@@ -649,7 +696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.2</v>
       </c>
@@ -661,7 +708,7 @@
       </c>
       <c r="D7" s="4"/>
       <c r="F7" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E7)),"Closed",IF(NOT(ISBLANK(D7)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H7" s="1" t="s">
@@ -671,7 +718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.2</v>
       </c>
@@ -683,7 +730,7 @@
       </c>
       <c r="D8" s="4"/>
       <c r="F8" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E8)),"Closed",IF(NOT(ISBLANK(D8)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H8" s="1" t="s">
@@ -693,25 +740,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>0.2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E9)),"Closed",IF(NOT(ISBLANK(D9)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G9" s="6">
         <v>43861</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.3</v>
       </c>
@@ -722,113 +769,131 @@
         <v>44170</v>
       </c>
       <c r="F10" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E10)),"Closed",IF(NOT(ISBLANK(D10)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>0.3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E11)),"Closed",IF(NOT(ISBLANK(D11)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G11" s="6">
         <v>43921</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="F12" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E12)),"Closed",IF(NOT(ISBLANK(D12)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F13" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E13)),"Closed",IF(NOT(ISBLANK(D13)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F14" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E14)),"Closed",IF(NOT(ISBLANK(D14)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F15" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E15)),"Closed",IF(NOT(ISBLANK(D15)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F16" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E16)),"Closed",IF(NOT(ISBLANK(D16)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E17)),"Closed",IF(NOT(ISBLANK(D17)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E18)),"Closed",IF(NOT(ISBLANK(D18)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E19)),"Closed",IF(NOT(ISBLANK(D19)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E20)),"Closed",IF(NOT(ISBLANK(D20)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E21)),"Closed",IF(NOT(ISBLANK(D21)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E22)),"Closed",IF(NOT(ISBLANK(D22)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E23)),"Closed",IF(NOT(ISBLANK(D23)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E24)),"Closed",IF(NOT(ISBLANK(D24)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E25)),"Closed",IF(NOT(ISBLANK(D25)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -839,6 +904,14 @@
       <sortCondition ref="B2:B25"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="J10" r:id="rId1" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
+    <hyperlink ref="K10" r:id="rId2" xr:uid="{E20F1CF4-A5E5-477C-916D-8D93441966B4}"/>
+    <hyperlink ref="L10" r:id="rId3" xr:uid="{EB3AF600-046C-4CF4-A630-32897A402939}"/>
+    <hyperlink ref="K11" r:id="rId4" xr:uid="{A526D1DE-B81B-41F4-8EAB-23F698FE0207}"/>
+    <hyperlink ref="J11" r:id="rId5" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
+    <hyperlink ref="L11" r:id="rId6" xr:uid="{2F9D6310-65D9-4024-84F7-8AB50095A431}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
better attr matching, create explore feateng
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B714867-65A5-4A1D-8DCF-27E64A476D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE662DD-D045-4A85-A531-28C3408B5DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>File/Line</t>
   </si>
@@ -45,9 +45,6 @@
     <t>b</t>
   </si>
   <si>
-    <t>add other attributes, e.g. market variables</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -124,6 +121,12 @@
   </si>
   <si>
     <t>https://github.com/romanorac/pandas-analytics-server</t>
+  </si>
+  <si>
+    <t>add other attributes, e.g. market variables, added one, to add more later</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more mkt variables </t>
   </si>
 </sst>
 </file>
@@ -182,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -206,6 +209,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -523,13 +529,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E7739-8A07-4817-ADF7-CBF975C125FD}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -551,25 +557,25 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
@@ -578,13 +584,13 @@
         <v>0</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -599,7 +605,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="F2" s="5" t="str">
-        <f t="shared" ref="F2:F25" si="0">IF(NOT(ISBLANK(E2)),"Closed",IF(NOT(ISBLANK(D2)),"In Progress",""))</f>
+        <f t="shared" ref="F2:F26" si="0">IF(NOT(ISBLANK(E2)),"Closed",IF(NOT(ISBLANK(D2)),"In Progress",""))</f>
         <v/>
       </c>
       <c r="H2" s="1" t="s">
@@ -609,7 +615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -622,12 +628,15 @@
       <c r="D3" s="4">
         <v>44180</v>
       </c>
+      <c r="E3" s="4">
+        <v>44185</v>
+      </c>
       <c r="F3" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
+        <v>Closed</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
@@ -649,7 +658,7 @@
         <v/>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -657,7 +666,7 @@
         <v>0.1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6">
@@ -671,29 +680,24 @@
         <v>44196</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.2</v>
       </c>
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4">
-        <v>44163</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>6</v>
+      <c r="B6" s="7">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9">
+        <v>44185</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -701,10 +705,10 @@
         <v>0.2</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4">
-        <v>44170</v>
+        <v>44163</v>
       </c>
       <c r="D7" s="4"/>
       <c r="F7" s="5" t="str">
@@ -712,10 +716,10 @@
         <v/>
       </c>
       <c r="H7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -723,7 +727,7 @@
         <v>0.2</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <v>44170</v>
@@ -734,92 +738,108 @@
         <v/>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="C9" s="4">
+        <v>44170</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="F9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>0.2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G10" s="6">
+        <v>43861</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4">
+        <v>44170</v>
+      </c>
+      <c r="F11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G9" s="6">
-        <v>43861</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="K11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4">
-        <v>44170</v>
-      </c>
-      <c r="F10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G11" s="6">
+      <c r="F12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G12" s="6">
         <v>43921</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="L12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="F12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
       <c r="F13" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -897,20 +917,26 @@
         <v/>
       </c>
     </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J25" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J25">
-      <sortCondition ref="A2:A25"/>
-      <sortCondition ref="B2:B25"/>
+  <autoFilter ref="A1:J26" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J26">
+      <sortCondition ref="A2:A26"/>
+      <sortCondition ref="B2:B26"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
-    <hyperlink ref="K10" r:id="rId2" xr:uid="{E20F1CF4-A5E5-477C-916D-8D93441966B4}"/>
-    <hyperlink ref="L10" r:id="rId3" xr:uid="{EB3AF600-046C-4CF4-A630-32897A402939}"/>
-    <hyperlink ref="K11" r:id="rId4" xr:uid="{A526D1DE-B81B-41F4-8EAB-23F698FE0207}"/>
-    <hyperlink ref="J11" r:id="rId5" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
-    <hyperlink ref="L11" r:id="rId6" xr:uid="{2F9D6310-65D9-4024-84F7-8AB50095A431}"/>
+    <hyperlink ref="J11" r:id="rId1" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
+    <hyperlink ref="K11" r:id="rId2" xr:uid="{E20F1CF4-A5E5-477C-916D-8D93441966B4}"/>
+    <hyperlink ref="L11" r:id="rId3" xr:uid="{EB3AF600-046C-4CF4-A630-32897A402939}"/>
+    <hyperlink ref="K12" r:id="rId4" xr:uid="{A526D1DE-B81B-41F4-8EAB-23F698FE0207}"/>
+    <hyperlink ref="J12" r:id="rId5" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
+    <hyperlink ref="L12" r:id="rId6" xr:uid="{2F9D6310-65D9-4024-84F7-8AB50095A431}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add notebook, update tracking
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA4853E-2B60-4784-A1A9-FA97B646D111}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3549CB0E-A28C-43DD-A08C-B2FAFDA528E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2955" yWindow="795" windowWidth="21120" windowHeight="13545" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
@@ -562,10 +562,10 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
start docker container, website not working
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133F4E01-02AB-4E71-9D46-C2806E16237C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA046DB-4977-41E2-BE4C-127AF19BA35D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
@@ -18,12 +18,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
     <definedName name="Z_0ABBB8F1_4417_4A6F_8334_B67935856E75_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
+    <definedName name="Z_3EB47DF6_EB2C_4BDE_A591_FB5D44A7319C_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
     <definedName name="Z_D2EEC5CB_748B_45CC_B066_739F6E799F2E_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All" guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1058" activeSheetId="1"/>
     <customWorkbookView name="Priorities" guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="All" guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1058" activeSheetId="1"/>
+    <customWorkbookView name="Open" guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>File/Line</t>
   </si>
@@ -172,6 +174,15 @@
   </si>
   <si>
     <t>Comment4</t>
+  </si>
+  <si>
+    <t>Running Docker Container With Gunicorn and Flask - DEV Community</t>
+  </si>
+  <si>
+    <t>https://deepu.tech/deploy-a-web-app-to-azure-app-service-using-terraform/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/azure/devops/pipelines/apps/cd/deploy-docker-webapp?view=azure-devops&amp;tabs=java</t>
   </si>
 </sst>
 </file>
@@ -230,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -262,6 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,7 +595,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -829,6 +841,7 @@
       <c r="H8" s="7" t="s">
         <v>39</v>
       </c>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -841,9 +854,12 @@
         <v>44170</v>
       </c>
       <c r="D9" s="4"/>
+      <c r="E9" s="4">
+        <v>44219</v>
+      </c>
       <c r="F9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Closed</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>35</v>
@@ -851,7 +867,10 @@
       <c r="I9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -870,6 +889,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="G10" s="4">
+        <v>44227</v>
+      </c>
       <c r="H10" s="1" t="s">
         <v>44</v>
       </c>
@@ -992,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.2</v>
       </c>
@@ -1009,8 +1031,12 @@
       <c r="H16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="J16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1173,6 +1199,12 @@
   </sheetData>
   <autoFilter ref="A1:J33" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}"/>
   <customSheetViews>
+    <customSheetView guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" showAutoFilter="1">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:J31" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+    </customSheetView>
     <customSheetView guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" filter="1" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
@@ -1194,11 +1226,15 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" showAutoFilter="1">
+    <customSheetView guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" filter="1" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J31" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+      <autoFilter ref="A1:J33" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <filterColumn colId="5">
+          <filters blank="1"/>
+        </filterColumn>
+      </autoFilter>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
@@ -1211,6 +1247,9 @@
     <hyperlink ref="L10" r:id="rId7" xr:uid="{84CE81F3-5CEE-4E2E-9A5A-C03CC54D4F13}"/>
     <hyperlink ref="J10" r:id="rId8" xr:uid="{287E5C28-FC49-46C9-8233-D49ECC1DDB77}"/>
     <hyperlink ref="M10" r:id="rId9" xr:uid="{4C15EAC7-467B-4588-844F-D7C03E34BC99}"/>
+    <hyperlink ref="J9" r:id="rId10" display="https://dev.to/marounmaroun/running-docker-container-with-gunicorn-and-flask-4ihg" xr:uid="{24866141-67C3-47E2-AEB0-0FBFAEAE9F8E}"/>
+    <hyperlink ref="J16" r:id="rId11" xr:uid="{F9D83654-F9A4-4D5C-B7A8-91BF2EB8176B}"/>
+    <hyperlink ref="K16" r:id="rId12" xr:uid="{F694B4BB-C22C-4CE5-B65E-8717DB82C2C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sample tic tac toe app
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA046DB-4977-41E2-BE4C-127AF19BA35D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD8EA88-6AE9-4975-8F04-627DD593FECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
+    <workbookView xWindow="2955" yWindow="795" windowWidth="23040" windowHeight="14235" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="architecture" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
-    <definedName name="Z_0ABBB8F1_4417_4A6F_8334_B67935856E75_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
-    <definedName name="Z_3EB47DF6_EB2C_4BDE_A591_FB5D44A7319C_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
-    <definedName name="Z_D2EEC5CB_748B_45CC_B066_739F6E799F2E_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
+    <definedName name="Z_0ABBB8F1_4417_4A6F_8334_B67935856E75_.wvu.FilterData" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
+    <definedName name="Z_3EB47DF6_EB2C_4BDE_A591_FB5D44A7319C_.wvu.FilterData" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
+    <definedName name="Z_D2EEC5CB_748B_45CC_B066_739F6E799F2E_.wvu.FilterData" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>File/Line</t>
   </si>
@@ -158,9 +159,6 @@
     <t>finish model selection pipeline</t>
   </si>
   <si>
-    <t>https://developer.okta.com/blog/2018/12/20/crud-app-with-python-flask-react</t>
-  </si>
-  <si>
     <t>https://react-jsonschema-form.readthedocs.io/en/latest/</t>
   </si>
   <si>
@@ -183,13 +181,79 @@
   </si>
   <si>
     <t>https://docs.microsoft.com/en-us/azure/devops/pipelines/apps/cd/deploy-docker-webapp?view=azure-devops&amp;tabs=java</t>
+  </si>
+  <si>
+    <t>https://amlanscloud.com/reactappdeploy/</t>
+  </si>
+  <si>
+    <t>https://github.com/ahmedbesbes/React-App-Flask-SSL</t>
+  </si>
+  <si>
+    <t>https://medium.com/swlh/deploy-and-secure-a-react-flask-app-with-docker-and-nginx-768ca582863b</t>
+  </si>
+  <si>
+    <t>https://tiangolo.medium.com/react-in-docker-with-nginx-built-with-multi-stage-docker-builds-including-testing-8cc49d6ec305</t>
+  </si>
+  <si>
+    <t>Backend (with analysis)</t>
+  </si>
+  <si>
+    <t>append market data</t>
+  </si>
+  <si>
+    <t>read in portfolio from IB</t>
+  </si>
+  <si>
+    <t>append own charactierstics</t>
+  </si>
+  <si>
+    <t>build model</t>
+  </si>
+  <si>
+    <t>build models</t>
+  </si>
+  <si>
+    <t>decide best model</t>
+  </si>
+  <si>
+    <t>Front end</t>
+  </si>
+  <si>
+    <t>read in csv file w characteristics</t>
+  </si>
+  <si>
+    <t>return model to user?</t>
+  </si>
+  <si>
+    <t>also allow someone to input model pickle + inputs</t>
+  </si>
+  <si>
+    <t>run model</t>
+  </si>
+  <si>
+    <t>run shap summary</t>
+  </si>
+  <si>
+    <t>show inputs</t>
+  </si>
+  <si>
+    <t>pickle file &amp; show inputs via mlflow</t>
+  </si>
+  <si>
+    <t>force plot</t>
+  </si>
+  <si>
+    <t>validation exhibits</t>
+  </si>
+  <si>
+    <t>Tutorial: Intro to React – React (reactjs.org)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +273,23 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -270,10 +351,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -589,13 +672,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E7739-8A07-4817-ADF7-CBF975C125FD}">
-  <dimension ref="A1:M33"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -613,10 +697,14 @@
     <col min="11" max="11" width="31.7109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="28.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="40" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="35.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="41.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="35.28515625" style="1" customWidth="1"/>
+    <col min="17" max="20" width="32.7109375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -654,10 +742,10 @@
         <v>24</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.1</v>
       </c>
@@ -684,7 +772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -708,7 +796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.1</v>
       </c>
@@ -735,7 +823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.1</v>
       </c>
@@ -765,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.1</v>
       </c>
@@ -792,7 +880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.1</v>
       </c>
@@ -817,7 +905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0.2</v>
       </c>
@@ -841,9 +929,9 @@
       <c r="H8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.2</v>
       </c>
@@ -868,13 +956,13 @@
         <v>5</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.2</v>
       </c>
@@ -884,99 +972,118 @@
       <c r="C10" s="4">
         <v>44219</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>44233</v>
+      </c>
       <c r="F10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>In Progress</v>
       </c>
       <c r="G10" s="4">
         <v>44227</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    </row>
+    <row r="11" spans="1:17" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>0.2</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="1">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4">
+        <v>44207</v>
+      </c>
+      <c r="F11" s="5" t="str">
+        <f>IF(NOT(ISBLANK(E11)),"Closed",IF(NOT(ISBLANK(D11)),"In Progress",""))</f>
+        <v/>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C12" s="9">
         <v>44185</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="F11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7" t="s">
+      <c r="D12" s="6"/>
+      <c r="F12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4">
-        <v>44170</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="F12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.2</v>
       </c>
       <c r="B13" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C13" s="4">
-        <v>44192</v>
+        <v>44170</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
       <c r="F13" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G13" s="4"/>
       <c r="H13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.2</v>
       </c>
       <c r="B14" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4">
         <v>44192</v>
@@ -989,55 +1096,51 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.2</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4">
-        <v>44162</v>
+        <v>44192</v>
       </c>
       <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.2</v>
       </c>
       <c r="B16" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4">
-        <v>44207</v>
-      </c>
+        <v>44162</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="F16" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="L16" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -1057,7 +1160,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.3</v>
       </c>
@@ -1111,93 +1214,104 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="F20" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F21" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F23" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F24" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F25" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F26" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F27" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F28" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F29" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F30" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F31" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="F32" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="F33" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J33" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}"/>
+  <autoFilter ref="A1:J33" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}">
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="In Progress"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <customSheetViews>
     <customSheetView guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -1238,19 +1352,178 @@
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="J18" r:id="rId1" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
-    <hyperlink ref="K18" r:id="rId2" xr:uid="{E20F1CF4-A5E5-477C-916D-8D93441966B4}"/>
-    <hyperlink ref="L18" r:id="rId3" xr:uid="{EB3AF600-046C-4CF4-A630-32897A402939}"/>
-    <hyperlink ref="K19" r:id="rId4" xr:uid="{A526D1DE-B81B-41F4-8EAB-23F698FE0207}"/>
-    <hyperlink ref="J19" r:id="rId5" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
-    <hyperlink ref="L19" r:id="rId6" xr:uid="{2F9D6310-65D9-4024-84F7-8AB50095A431}"/>
-    <hyperlink ref="L10" r:id="rId7" xr:uid="{84CE81F3-5CEE-4E2E-9A5A-C03CC54D4F13}"/>
-    <hyperlink ref="J10" r:id="rId8" xr:uid="{287E5C28-FC49-46C9-8233-D49ECC1DDB77}"/>
-    <hyperlink ref="M10" r:id="rId9" xr:uid="{4C15EAC7-467B-4588-844F-D7C03E34BC99}"/>
-    <hyperlink ref="J9" r:id="rId10" display="https://dev.to/marounmaroun/running-docker-container-with-gunicorn-and-flask-4ihg" xr:uid="{24866141-67C3-47E2-AEB0-0FBFAEAE9F8E}"/>
-    <hyperlink ref="J16" r:id="rId11" xr:uid="{F9D83654-F9A4-4D5C-B7A8-91BF2EB8176B}"/>
-    <hyperlink ref="K16" r:id="rId12" xr:uid="{F694B4BB-C22C-4CE5-B65E-8717DB82C2C1}"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{E20F1CF4-A5E5-477C-916D-8D93441966B4}"/>
+    <hyperlink ref="L18" r:id="rId2" xr:uid="{EB3AF600-046C-4CF4-A630-32897A402939}"/>
+    <hyperlink ref="K19" r:id="rId3" xr:uid="{A526D1DE-B81B-41F4-8EAB-23F698FE0207}"/>
+    <hyperlink ref="L19" r:id="rId4" xr:uid="{2F9D6310-65D9-4024-84F7-8AB50095A431}"/>
+    <hyperlink ref="J9" r:id="rId5" display="https://dev.to/marounmaroun/running-docker-container-with-gunicorn-and-flask-4ihg" xr:uid="{24866141-67C3-47E2-AEB0-0FBFAEAE9F8E}"/>
+    <hyperlink ref="K11" r:id="rId6" xr:uid="{F694B4BB-C22C-4CE5-B65E-8717DB82C2C1}"/>
+    <hyperlink ref="M10" r:id="rId7" xr:uid="{0C32E2FA-D722-41D8-A3F6-1DB3FCFD511F}"/>
+    <hyperlink ref="N10" r:id="rId8" xr:uid="{93DC91F2-0F1B-4C59-9650-83EB444D8B52}"/>
+    <hyperlink ref="Q10" r:id="rId9" xr:uid="{F2E1004F-471F-43B8-A1E8-AEF6A223B0E8}"/>
+    <hyperlink ref="O10" r:id="rId10" xr:uid="{3D4AB481-4DFD-43F4-9962-FE73EE10FA0D}"/>
+    <hyperlink ref="P10" r:id="rId11" xr:uid="{1115D1A6-B3ED-4462-B38E-81A90380E4E4}"/>
+    <hyperlink ref="K10" r:id="rId12" xr:uid="{730FDAEF-3D20-4A3A-858F-091DE2CE9230}"/>
+    <hyperlink ref="L10" r:id="rId13" xr:uid="{966DA437-8ABC-4AE2-B482-4C6FA4D690E3}"/>
+    <hyperlink ref="J11" r:id="rId14" xr:uid="{F9D83654-F9A4-4D5C-B7A8-91BF2EB8176B}"/>
+    <hyperlink ref="J19" r:id="rId15" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
+    <hyperlink ref="J18" r:id="rId16" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
+    <hyperlink ref="J10" r:id="rId17" location="adding-time-travel" display="https://reactjs.org/tutorial/tutorial.html - adding-time-travel" xr:uid="{7DDEAA13-ECD9-4465-BA88-3631E0F66777}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E282F770-B431-4101-8D5E-3BD9FAB51E57}">
+  <dimension ref="B2:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix readme and tracking
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD8EA88-6AE9-4975-8F04-627DD593FECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6432C0BE-32DD-4A31-805B-4802A6AE3DBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="795" windowWidth="23040" windowHeight="14235" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="architecture" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
@@ -24,9 +23,9 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Open" guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Priorities" guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="All" guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1058" activeSheetId="1"/>
-    <customWorkbookView name="Priorities" guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Open" guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>File/Line</t>
   </si>
@@ -193,57 +192,6 @@
   </si>
   <si>
     <t>https://tiangolo.medium.com/react-in-docker-with-nginx-built-with-multi-stage-docker-builds-including-testing-8cc49d6ec305</t>
-  </si>
-  <si>
-    <t>Backend (with analysis)</t>
-  </si>
-  <si>
-    <t>append market data</t>
-  </si>
-  <si>
-    <t>read in portfolio from IB</t>
-  </si>
-  <si>
-    <t>append own charactierstics</t>
-  </si>
-  <si>
-    <t>build model</t>
-  </si>
-  <si>
-    <t>build models</t>
-  </si>
-  <si>
-    <t>decide best model</t>
-  </si>
-  <si>
-    <t>Front end</t>
-  </si>
-  <si>
-    <t>read in csv file w characteristics</t>
-  </si>
-  <si>
-    <t>return model to user?</t>
-  </si>
-  <si>
-    <t>also allow someone to input model pickle + inputs</t>
-  </si>
-  <si>
-    <t>run model</t>
-  </si>
-  <si>
-    <t>run shap summary</t>
-  </si>
-  <si>
-    <t>show inputs</t>
-  </si>
-  <si>
-    <t>pickle file &amp; show inputs via mlflow</t>
-  </si>
-  <si>
-    <t>force plot</t>
-  </si>
-  <si>
-    <t>validation exhibits</t>
   </si>
   <si>
     <t>Tutorial: Intro to React – React (reactjs.org)</t>
@@ -253,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,23 +221,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -322,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -355,8 +286,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -672,14 +601,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E7739-8A07-4817-ADF7-CBF975C125FD}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -745,7 +673,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.1</v>
       </c>
@@ -772,7 +700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -796,7 +724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.1</v>
       </c>
@@ -823,7 +751,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.1</v>
       </c>
@@ -853,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.1</v>
       </c>
@@ -880,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.1</v>
       </c>
@@ -905,7 +833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0.2</v>
       </c>
@@ -931,7 +859,7 @@
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.2</v>
       </c>
@@ -986,7 +914,7 @@
         <v>43</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>41</v>
@@ -1010,7 +938,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.2</v>
       </c>
@@ -1035,7 +963,7 @@
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>0.2</v>
       </c>
@@ -1056,7 +984,7 @@
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.2</v>
       </c>
@@ -1078,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.2</v>
       </c>
@@ -1099,7 +1027,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.2</v>
       </c>
@@ -1120,7 +1048,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.2</v>
       </c>
@@ -1160,7 +1088,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.3</v>
       </c>
@@ -1214,110 +1142,103 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="F20" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F21" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F23" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F24" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F25" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F26" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F27" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F28" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F29" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F30" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F31" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F32" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J33" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}">
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="In Progress"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J33" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}"/>
   <customSheetViews>
-    <customSheetView guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" showAutoFilter="1">
+    <customSheetView guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" filter="1" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J31" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+      <autoFilter ref="A1:J33" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <filterColumn colId="5">
+          <filters blank="1"/>
+        </filterColumn>
+      </autoFilter>
     </customSheetView>
     <customSheetView guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" filter="1" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -1340,15 +1261,11 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J33" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <filterColumn colId="5">
-          <filters blank="1"/>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="A1:J31" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
@@ -1372,158 +1289,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E282F770-B431-4101-8D5E-3BD9FAB51E57}">
-  <dimension ref="B2:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
re remove mlruns and update plots
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6432C0BE-32DD-4A31-805B-4802A6AE3DBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95BFF42-F3CC-4949-B8CB-10DE26296CDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="keyinsights" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
     <definedName name="Z_0ABBB8F1_4417_4A6F_8334_B67935856E75_.wvu.FilterData" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
-    <definedName name="Z_3EB47DF6_EB2C_4BDE_A591_FB5D44A7319C_.wvu.FilterData" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
+    <definedName name="Z_3CA5A9AE_04CF_4338_A1D5_B449182FE622_.wvu.FilterData" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
     <definedName name="Z_D2EEC5CB_748B_45CC_B066_739F6E799F2E_.wvu.FilterData" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Open" guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Priorities" guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="All" guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1058" activeSheetId="1"/>
+    <customWorkbookView name="Open" guid="{3CA5A9AE-04CF-4338-A1D5-B449182FE622}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>File/Line</t>
   </si>
@@ -195,6 +196,18 @@
   </si>
   <si>
     <t>Tutorial: Intro to React – React (reactjs.org)</t>
+  </si>
+  <si>
+    <t>swap scoring with dependence plots</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>vix &gt; 35 is reliable for gains</t>
   </si>
 </sst>
 </file>
@@ -253,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +299,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -601,13 +615,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E7739-8A07-4817-ADF7-CBF975C125FD}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="15" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -673,7 +688,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.1</v>
       </c>
@@ -700,7 +715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -724,75 +739,75 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.1</v>
       </c>
       <c r="B4" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4">
-        <v>44191</v>
+        <v>44163</v>
       </c>
       <c r="D4" s="4">
         <v>44196</v>
       </c>
       <c r="E4" s="4">
-        <v>44213</v>
+        <v>44198</v>
       </c>
       <c r="F4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G4" s="4">
-        <v>44203</v>
+        <v>44194</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.1</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4">
-        <v>44163</v>
+        <v>44191</v>
       </c>
       <c r="D5" s="4">
-        <v>44196</v>
+        <v>44213</v>
       </c>
       <c r="E5" s="4">
-        <v>44198</v>
+        <v>44213</v>
       </c>
       <c r="F5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G5" s="4">
-        <v>44194</v>
+        <v>44216</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.1</v>
       </c>
       <c r="B6" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="4">
         <v>44191</v>
       </c>
       <c r="D6" s="4">
-        <v>44213</v>
+        <v>44196</v>
       </c>
       <c r="E6" s="4">
         <v>44213</v>
@@ -802,13 +817,13 @@
         <v>Closed</v>
       </c>
       <c r="G6" s="4">
-        <v>44216</v>
+        <v>44203</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.1</v>
       </c>
@@ -833,33 +848,39 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+    <row r="8" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>0.2</v>
       </c>
-      <c r="B8" s="7">
-        <v>14</v>
-      </c>
-      <c r="C8" s="9">
-        <v>44517</v>
-      </c>
-      <c r="D8" s="9">
-        <v>44219</v>
-      </c>
-      <c r="E8" s="9">
-        <v>44219</v>
-      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>44162</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Closed</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.2</v>
       </c>
@@ -890,250 +911,303 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.2</v>
       </c>
       <c r="B10" s="1">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4">
-        <v>44219</v>
-      </c>
-      <c r="D10" s="4">
-        <v>44233</v>
-      </c>
+        <v>44170</v>
+      </c>
+      <c r="D10" s="4"/>
       <c r="F10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
-      </c>
-      <c r="G10" s="4">
-        <v>44227</v>
+        <v/>
       </c>
       <c r="H10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.2</v>
       </c>
-      <c r="B11" s="1">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4">
-        <v>44207</v>
-      </c>
+      <c r="B11" s="7">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9">
+        <v>44185</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E11)),"Closed",IF(NOT(ISBLANK(D11)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>0.2</v>
       </c>
-      <c r="B12" s="7">
-        <v>8</v>
-      </c>
-      <c r="C12" s="9">
-        <v>44185</v>
-      </c>
-      <c r="D12" s="6"/>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4">
+        <v>44192</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G12" s="4"/>
+      <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.2</v>
       </c>
       <c r="B13" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4">
-        <v>44170</v>
+        <v>44192</v>
       </c>
       <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.2</v>
       </c>
       <c r="B14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4">
-        <v>44192</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+        <v>44207</v>
+      </c>
       <c r="F14" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G14" s="4"/>
       <c r="H14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+        <v>34</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>0.2</v>
       </c>
-      <c r="B15" s="1">
-        <v>11</v>
-      </c>
-      <c r="C15" s="4">
-        <v>44192</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="7">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9">
+        <v>44517</v>
+      </c>
+      <c r="D15" s="9">
+        <v>44219</v>
+      </c>
+      <c r="E15" s="9">
+        <v>44219</v>
+      </c>
       <c r="F15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>Closed</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.2</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C16" s="4">
-        <v>44162</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>44219</v>
+      </c>
+      <c r="D16" s="4">
+        <v>44233</v>
+      </c>
       <c r="F16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>In Progress</v>
+      </c>
+      <c r="G16" s="4">
+        <v>44314</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+        <v>43</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>0.2</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G17" s="4">
+        <v>44314</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G17" s="6">
-        <v>44286</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G18" s="6">
+        <v>44347</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>0.3</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>7</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C19" s="4">
         <v>44170</v>
       </c>
-      <c r="F18" s="5" t="str">
-        <f t="shared" ref="F18:F19" si="1">IF(NOT(ISBLANK(E18)),"Closed",IF(NOT(ISBLANK(D18)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="I19" s="1"/>
+      <c r="J19" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G19" s="6">
-        <v>44377</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>25</v>
@@ -1142,104 +1216,146 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
       <c r="F20" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G20" s="6">
+        <v>44377</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>17</v>
+      </c>
       <c r="F21" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>18</v>
+      </c>
       <c r="F22" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>19</v>
+      </c>
       <c r="F23" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>20</v>
+      </c>
       <c r="F24" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>21</v>
+      </c>
       <c r="F25" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>22</v>
+      </c>
       <c r="F26" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="F27" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="F28" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="F29" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="F30" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="F31" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="F32" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="F33" s="5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J33" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}"/>
+  <autoFilter ref="A1:J33" xr:uid="{0F7B0E99-896E-4BA5-929F-442168AC0038}">
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="In Progress"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:Q33">
+    <sortCondition ref="A2:A33"/>
+    <sortCondition ref="B2:B33"/>
+    <sortCondition descending="1" ref="G2:G33"/>
+  </sortState>
   <customSheetViews>
-    <customSheetView guid="{3EB47DF6-EB2C-4BDE-A591-FB5D44A7319C}" filter="1" showAutoFilter="1">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J33" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <filterColumn colId="5">
-          <filters blank="1"/>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
     <customSheetView guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" filter="1" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
@@ -1267,26 +1383,72 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:J31" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
+    <customSheetView guid="{3CA5A9AE-04CF-4338-A1D5-B449182FE622}" filter="1" showAutoFilter="1">
+      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:J33" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <filterColumn colId="5">
+          <filters blank="1">
+            <filter val="In Progress"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
   </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{E20F1CF4-A5E5-477C-916D-8D93441966B4}"/>
-    <hyperlink ref="L18" r:id="rId2" xr:uid="{EB3AF600-046C-4CF4-A630-32897A402939}"/>
+    <hyperlink ref="K17" r:id="rId1" xr:uid="{E20F1CF4-A5E5-477C-916D-8D93441966B4}"/>
+    <hyperlink ref="L17" r:id="rId2" xr:uid="{EB3AF600-046C-4CF4-A630-32897A402939}"/>
     <hyperlink ref="K19" r:id="rId3" xr:uid="{A526D1DE-B81B-41F4-8EAB-23F698FE0207}"/>
     <hyperlink ref="L19" r:id="rId4" xr:uid="{2F9D6310-65D9-4024-84F7-8AB50095A431}"/>
     <hyperlink ref="J9" r:id="rId5" display="https://dev.to/marounmaroun/running-docker-container-with-gunicorn-and-flask-4ihg" xr:uid="{24866141-67C3-47E2-AEB0-0FBFAEAE9F8E}"/>
-    <hyperlink ref="K11" r:id="rId6" xr:uid="{F694B4BB-C22C-4CE5-B65E-8717DB82C2C1}"/>
-    <hyperlink ref="M10" r:id="rId7" xr:uid="{0C32E2FA-D722-41D8-A3F6-1DB3FCFD511F}"/>
-    <hyperlink ref="N10" r:id="rId8" xr:uid="{93DC91F2-0F1B-4C59-9650-83EB444D8B52}"/>
-    <hyperlink ref="Q10" r:id="rId9" xr:uid="{F2E1004F-471F-43B8-A1E8-AEF6A223B0E8}"/>
-    <hyperlink ref="O10" r:id="rId10" xr:uid="{3D4AB481-4DFD-43F4-9962-FE73EE10FA0D}"/>
-    <hyperlink ref="P10" r:id="rId11" xr:uid="{1115D1A6-B3ED-4462-B38E-81A90380E4E4}"/>
-    <hyperlink ref="K10" r:id="rId12" xr:uid="{730FDAEF-3D20-4A3A-858F-091DE2CE9230}"/>
-    <hyperlink ref="L10" r:id="rId13" xr:uid="{966DA437-8ABC-4AE2-B482-4C6FA4D690E3}"/>
-    <hyperlink ref="J11" r:id="rId14" xr:uid="{F9D83654-F9A4-4D5C-B7A8-91BF2EB8176B}"/>
-    <hyperlink ref="J19" r:id="rId15" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
-    <hyperlink ref="J18" r:id="rId16" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
-    <hyperlink ref="J10" r:id="rId17" location="adding-time-travel" display="https://reactjs.org/tutorial/tutorial.html - adding-time-travel" xr:uid="{7DDEAA13-ECD9-4465-BA88-3631E0F66777}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{F694B4BB-C22C-4CE5-B65E-8717DB82C2C1}"/>
+    <hyperlink ref="M16" r:id="rId7" xr:uid="{0C32E2FA-D722-41D8-A3F6-1DB3FCFD511F}"/>
+    <hyperlink ref="N16" r:id="rId8" xr:uid="{93DC91F2-0F1B-4C59-9650-83EB444D8B52}"/>
+    <hyperlink ref="Q16" r:id="rId9" xr:uid="{F2E1004F-471F-43B8-A1E8-AEF6A223B0E8}"/>
+    <hyperlink ref="O16" r:id="rId10" xr:uid="{3D4AB481-4DFD-43F4-9962-FE73EE10FA0D}"/>
+    <hyperlink ref="P16" r:id="rId11" xr:uid="{1115D1A6-B3ED-4462-B38E-81A90380E4E4}"/>
+    <hyperlink ref="K16" r:id="rId12" xr:uid="{730FDAEF-3D20-4A3A-858F-091DE2CE9230}"/>
+    <hyperlink ref="L16" r:id="rId13" xr:uid="{966DA437-8ABC-4AE2-B482-4C6FA4D690E3}"/>
+    <hyperlink ref="J14" r:id="rId14" xr:uid="{F9D83654-F9A4-4D5C-B7A8-91BF2EB8176B}"/>
+    <hyperlink ref="J20" r:id="rId15" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
+    <hyperlink ref="J19" r:id="rId16" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
+    <hyperlink ref="J16" r:id="rId17" location="adding-time-travel" display="https://reactjs.org/tutorial/tutorial.html - adding-time-travel" xr:uid="{7DDEAA13-ECD9-4465-BA88-3631E0F66777}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E2D3BE-EB92-413D-A107-1187B4B36647}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>44296</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update readme & tracking
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43912E6B-3683-4DEB-8A62-25985FED39F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A824FC-9B08-4B61-9538-1C037C1A2A5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>File/Line</t>
   </si>
@@ -207,7 +207,13 @@
     <t>result</t>
   </si>
   <si>
-    <t>vix &gt; 35 is reliable for gains</t>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>per ML model w/ shap</t>
+  </si>
+  <si>
+    <t>vix &gt; 35 is reliable for long position gains</t>
   </si>
 </sst>
 </file>
@@ -622,7 +628,7 @@
       <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -705,7 +711,7 @@
         <v>44185</v>
       </c>
       <c r="F2" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E2)),"Closed",IF(NOT(ISBLANK(D2)),"In Progress",""))</f>
+        <f t="shared" ref="F2:F8" si="0">IF(NOT(ISBLANK(E2)),"Closed",IF(NOT(ISBLANK(D2)),"In Progress",""))</f>
         <v>Closed</v>
       </c>
       <c r="G2" s="4">
@@ -735,7 +741,7 @@
         <v>44191</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E3)),"Closed",IF(NOT(ISBLANK(D3)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G3" s="4">
@@ -762,7 +768,7 @@
         <v>44198</v>
       </c>
       <c r="F4" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E4)),"Closed",IF(NOT(ISBLANK(D4)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G4" s="4">
@@ -792,7 +798,7 @@
         <v>44213</v>
       </c>
       <c r="F5" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E5)),"Closed",IF(NOT(ISBLANK(D5)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G5" s="4">
@@ -819,7 +825,7 @@
         <v>44213</v>
       </c>
       <c r="F6" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E6)),"Closed",IF(NOT(ISBLANK(D6)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G6" s="4">
@@ -844,7 +850,7 @@
         <v>44219</v>
       </c>
       <c r="F7" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E7)),"Closed",IF(NOT(ISBLANK(D7)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G7" s="4">
@@ -875,7 +881,7 @@
         <v>44213</v>
       </c>
       <c r="F8" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E8)),"Closed",IF(NOT(ISBLANK(D8)),"In Progress",""))</f>
+        <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
       <c r="G8" s="6">
@@ -899,71 +905,78 @@
         <v>0.2</v>
       </c>
       <c r="B9" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C9" s="4">
-        <v>44219</v>
-      </c>
-      <c r="D9" s="4">
-        <v>44233</v>
-      </c>
+        <v>44162</v>
+      </c>
+      <c r="D9" s="4"/>
       <c r="F9" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E9)),"Closed",IF(NOT(ISBLANK(D9)),"In Progress",""))</f>
-        <v>In Progress</v>
+        <f t="shared" ref="F9:F33" si="1">IF(NOT(ISBLANK(E9)),"Closed",IF(NOT(ISBLANK(D9)),"In Progress",""))</f>
+        <v/>
       </c>
       <c r="G9" s="4">
-        <v>44314</v>
+        <v>44331</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>52</v>
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="1">
         <v>0.2</v>
       </c>
       <c r="B10" s="1">
-        <v>16</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C10" s="4">
+        <v>44192</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E10)),"Closed",IF(NOT(ISBLANK(D10)),"In Progress",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G10" s="4">
-        <v>44314</v>
+        <v>44331</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>0.2</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="1">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4">
+        <v>44219</v>
+      </c>
+      <c r="D11" s="4">
+        <v>44233</v>
+      </c>
       <c r="F11" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E11)),"Closed",IF(NOT(ISBLANK(D11)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="G11" s="6">
+        <f t="shared" si="1"/>
+        <v>In Progress</v>
+      </c>
+      <c r="G11" s="4">
         <v>44347</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="H11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="8"/>
@@ -972,26 +985,28 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E12)),"Closed",IF(NOT(ISBLANK(D12)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="G12" s="6">
-        <v>44377</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>26</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G12" s="4">
+        <v>44347</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1000,76 +1015,79 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>0.2</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <v>44162</v>
-      </c>
-      <c r="D13" s="4"/>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E13)),"Closed",IF(NOT(ISBLANK(D13)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="B14" s="1">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4">
-        <v>44170</v>
-      </c>
-      <c r="D14" s="4"/>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G13" s="6">
+        <v>44377</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E14)),"Closed",IF(NOT(ISBLANK(D14)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G14" s="6">
+        <v>44469</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>47</v>
       </c>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>0.2</v>
       </c>
-      <c r="B15" s="7">
-        <v>8</v>
-      </c>
-      <c r="C15" s="9">
-        <v>44185</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="1">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4">
+        <v>44170</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="F15" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E15)),"Closed",IF(NOT(ISBLANK(D15)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -1078,26 +1096,28 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>0.2</v>
       </c>
-      <c r="B16" s="1">
-        <v>11</v>
-      </c>
-      <c r="C16" s="4">
-        <v>44192</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="7">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9">
+        <v>44185</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E16)),"Closed",IF(NOT(ISBLANK(D16)),"In Progress",""))</f>
-        <v/>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="1" t="s">
-        <v>33</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="8" t="s">
         <v>41</v>
       </c>
@@ -1120,7 +1140,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="2" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.2</v>
       </c>
@@ -1133,7 +1153,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E17)),"Closed",IF(NOT(ISBLANK(D17)),"In Progress",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G17" s="4"/>
@@ -1154,7 +1174,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.2</v>
       </c>
@@ -1165,7 +1185,7 @@
         <v>44207</v>
       </c>
       <c r="F18" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E18)),"Closed",IF(NOT(ISBLANK(D18)),"In Progress",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H18" s="1" t="s">
@@ -1199,7 +1219,7 @@
         <v>44219</v>
       </c>
       <c r="F19" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E19)),"Closed",IF(NOT(ISBLANK(D19)),"In Progress",""))</f>
+        <f t="shared" si="1"/>
         <v>Closed</v>
       </c>
       <c r="G19" s="9"/>
@@ -1215,7 +1235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.3</v>
       </c>
@@ -1226,7 +1246,7 @@
         <v>44170</v>
       </c>
       <c r="F20" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E20)),"Closed",IF(NOT(ISBLANK(D20)),"In Progress",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H20" s="1" t="s">
@@ -1236,99 +1256,99 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>17</v>
       </c>
       <c r="F21" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E21)),"Closed",IF(NOT(ISBLANK(D21)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>18</v>
       </c>
       <c r="F22" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E22)),"Closed",IF(NOT(ISBLANK(D22)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>19</v>
       </c>
       <c r="F23" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E23)),"Closed",IF(NOT(ISBLANK(D23)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>20</v>
       </c>
       <c r="F24" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E24)),"Closed",IF(NOT(ISBLANK(D24)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>21</v>
       </c>
       <c r="F25" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E25)),"Closed",IF(NOT(ISBLANK(D25)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>22</v>
       </c>
       <c r="F26" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E26)),"Closed",IF(NOT(ISBLANK(D26)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F27" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E27)),"Closed",IF(NOT(ISBLANK(D27)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F28" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E28)),"Closed",IF(NOT(ISBLANK(D28)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F29" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E29)),"Closed",IF(NOT(ISBLANK(D29)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F30" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E30)),"Closed",IF(NOT(ISBLANK(D30)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F31" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E31)),"Closed",IF(NOT(ISBLANK(D31)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F32" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E32)),"Closed",IF(NOT(ISBLANK(D32)),"In Progress",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="6:6" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="5" t="str">
-        <f>IF(NOT(ISBLANK(E33)),"Closed",IF(NOT(ISBLANK(D33)),"In Progress",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1339,12 +1359,7 @@
         <filter val="In Progress"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J33">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:J33">
       <sortCondition ref="G1:G33"/>
     </sortState>
   </autoFilter>
@@ -1409,9 +1424,9 @@
     <hyperlink ref="K16" r:id="rId12" xr:uid="{730FDAEF-3D20-4A3A-858F-091DE2CE9230}"/>
     <hyperlink ref="L16" r:id="rId13" xr:uid="{966DA437-8ABC-4AE2-B482-4C6FA4D690E3}"/>
     <hyperlink ref="J18" r:id="rId14" xr:uid="{F9D83654-F9A4-4D5C-B7A8-91BF2EB8176B}"/>
-    <hyperlink ref="J12" r:id="rId15" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
+    <hyperlink ref="J14" r:id="rId15" xr:uid="{CBF38C8E-74EF-4F87-B3A7-18075F9E592F}"/>
     <hyperlink ref="J20" r:id="rId16" xr:uid="{37EE4BA1-F7ED-4BC3-B5CC-17469E90B3B6}"/>
-    <hyperlink ref="J9" r:id="rId17" location="adding-time-travel" display="https://reactjs.org/tutorial/tutorial.html - adding-time-travel" xr:uid="{7DDEAA13-ECD9-4465-BA88-3631E0F66777}"/>
+    <hyperlink ref="J11" r:id="rId17" location="adding-time-travel" display="https://reactjs.org/tutorial/tutorial.html - adding-time-travel" xr:uid="{7DDEAA13-ECD9-4465-BA88-3631E0F66777}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1419,31 +1434,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E2D3BE-EB92-413D-A107-1187B4B36647}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>44296</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add h2o test and update mlflow backend store
</commit_message>
<xml_diff>
--- a/P1-AnalyzeTrades/_Project-Tracking.xlsx
+++ b/P1-AnalyzeTrades/_Project-Tracking.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Important\CareerNCollege\AdHoc\Git\quant-trading\P1-AnalyzeTrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A824FC-9B08-4B61-9538-1C037C1A2A5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6579291E-3360-4878-AAFC-3F2926188697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
+    <workbookView xWindow="3795" yWindow="1275" windowWidth="21585" windowHeight="12960" xr2:uid="{6FE18BA9-7C93-4E0C-A4FC-D61FC48B25C1}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="keyinsights" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$J$33</definedName>
@@ -24,9 +23,9 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Priorities" guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="All" guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1058" activeSheetId="1"/>
     <customWorkbookView name="Open" guid="{3CA5A9AE-04CF-4338-A1D5-B449182FE622}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="All" guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1058" activeSheetId="1"/>
-    <customWorkbookView name="Priorities" guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>File/Line</t>
   </si>
@@ -199,21 +198,6 @@
   </si>
   <si>
     <t>swap scoring with dependence plots</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>reason</t>
-  </si>
-  <si>
-    <t>per ML model w/ shap</t>
-  </si>
-  <si>
-    <t>vix &gt; 35 is reliable for long position gains</t>
   </si>
 </sst>
 </file>
@@ -272,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -305,7 +289,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -628,7 +611,7 @@
       <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1369,29 +1352,11 @@
     <sortCondition descending="1" ref="G2:G33"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{3CA5A9AE-04CF-4338-A1D5-B449182FE622}" filter="1" showAutoFilter="1">
-      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J33" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <filterColumn colId="5">
-          <filters blank="1">
-            <filter val="In Progress"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" showAutoFilter="1">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J31" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
-    </customSheetView>
     <customSheetView guid="{0ABBB8F1-4417-4A6F-8334-B67935856E75}" filter="1" showAutoFilter="1">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J30" xr:uid="{00000000-0000-0000-0000-000000000000}">
+      <autoFilter ref="A1:J30" xr:uid="{13FE08FE-E30C-40CC-B357-69ABAE53646C}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="In Progress"/>
@@ -1406,6 +1371,24 @@
           <sortCondition ref="A2:A30"/>
           <sortCondition ref="B2:B30"/>
         </sortState>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{D2EEC5CB-748B-45CC-B066-739F6E799F2E}" showAutoFilter="1">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:J31" xr:uid="{ED0D04E5-8A35-493C-9BDA-E62CFAF69C99}"/>
+    </customSheetView>
+    <customSheetView guid="{3CA5A9AE-04CF-4338-A1D5-B449182FE622}" filter="1" showAutoFilter="1">
+      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:J33" xr:uid="{5160EDC5-4D49-4EE2-BCD1-2B70CD275D13}">
+        <filterColumn colId="5">
+          <filters blank="1">
+            <filter val="In Progress"/>
+          </filters>
+        </filterColumn>
       </autoFilter>
     </customSheetView>
   </customSheetViews>
@@ -1430,45 +1413,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E2D3BE-EB92-413D-A107-1187B4B36647}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>44296</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>